<commit_message>
Tweaks to biomass and updates to recapture analyssi.
</commit_message>
<xml_diff>
--- a/data/releases_v2.xlsx
+++ b/data/releases_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/smelt cages/Smelt-cages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{3A8690C5-4D70-4D7F-A720-A581899B766F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C870BCFE-9384-4335-A867-8BE2A604FB4A}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="8_{3A8690C5-4D70-4D7F-A720-A581899B766F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C4530D0-FA94-4B4C-8020-130D667415C5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{0D96B6DC-AD06-4C7E-9A7B-1DEB3E058018}"/>
+    <workbookView xWindow="29520" yWindow="480" windowWidth="19110" windowHeight="11235" xr2:uid="{0D96B6DC-AD06-4C7E-9A7B-1DEB3E058018}"/>
   </bookViews>
   <sheets>
     <sheet name="releases" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
   <si>
     <t>ReleaseEvent</t>
   </si>
@@ -187,19 +187,53 @@
   </si>
   <si>
     <t>FirstFlush</t>
+  </si>
+  <si>
+    <t>BY2024 1</t>
+  </si>
+  <si>
+    <t>BY2024 2</t>
+  </si>
+  <si>
+    <t>BY2024 3</t>
+  </si>
+  <si>
+    <t>BY2024 4</t>
+  </si>
+  <si>
+    <t>Lookout Slough</t>
+  </si>
+  <si>
+    <t>Sandy Beach</t>
+  </si>
+  <si>
+    <t>Left/Blue/AD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,10 +256,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E888D9-CA43-4314-8E40-1975A861CC6D}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1018,8 +1055,113 @@
         <v>-121.699521</v>
       </c>
     </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45614</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="2">
+        <v>13573</v>
+      </c>
+      <c r="G19" s="5">
+        <v>38.326289000000003</v>
+      </c>
+      <c r="H19" s="5">
+        <v>-121.69402599999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45635</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="4">
+        <v>14880</v>
+      </c>
+      <c r="G20" s="5">
+        <v>38.326289000000003</v>
+      </c>
+      <c r="H20" s="5">
+        <v>-121.69402599999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45644</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="4">
+        <v>20219</v>
+      </c>
+      <c r="G21">
+        <v>38.140123600000003</v>
+      </c>
+      <c r="H21">
+        <v>-121.694585365953</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45665</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="4">
+        <v>10024</v>
+      </c>
+      <c r="G22" s="5">
+        <v>38.326289000000003</v>
+      </c>
+      <c r="H22" s="5">
+        <v>-121.69402599999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1027,7 +1169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD554DC-4399-4643-A978-2B54083BE8FA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>